<commit_message>
changes for account enrichment service added
</commit_message>
<xml_diff>
--- a/cusaccount.xlsx
+++ b/cusaccount.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>Account Id</t>
   </si>
@@ -26,163 +26,178 @@
     <t>Balance Date</t>
   </si>
   <si>
+    <t>000000000009</t>
+  </si>
+  <si>
+    <t>Nazi Rure</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>2023-02-23</t>
+  </si>
+  <si>
+    <t>000000000010</t>
+  </si>
+  <si>
+    <t>Deze Quru</t>
+  </si>
+  <si>
+    <t>0.61</t>
+  </si>
+  <si>
+    <t>000000000011</t>
+  </si>
+  <si>
+    <t>Geka Tozo</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>000000000012</t>
+  </si>
+  <si>
+    <t>Raxo Lame</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>000000000013</t>
+  </si>
+  <si>
+    <t>Fono Woga</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>000000000014</t>
+  </si>
+  <si>
+    <t>Mexi Naso</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>000000000015</t>
+  </si>
+  <si>
+    <t>Vewa Voba</t>
+  </si>
+  <si>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>000000000016</t>
+  </si>
+  <si>
+    <t>Fodu Nuju</t>
+  </si>
+  <si>
+    <t>0.42</t>
+  </si>
+  <si>
+    <t>000000000017</t>
+  </si>
+  <si>
+    <t>Joqi Kewo</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>000000000018</t>
+  </si>
+  <si>
+    <t>Yeru Mowo</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>000000000001</t>
+  </si>
+  <si>
+    <t>abcd1</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>000000000019</t>
+  </si>
+  <si>
+    <t>Vime Juwa</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>000000000002</t>
+  </si>
+  <si>
+    <t>abcd2</t>
+  </si>
+  <si>
+    <t>0.53</t>
+  </si>
+  <si>
+    <t>000000000003</t>
+  </si>
+  <si>
+    <t>abcd3</t>
+  </si>
+  <si>
+    <t>0.44</t>
+  </si>
+  <si>
+    <t>000000000004</t>
+  </si>
+  <si>
+    <t>abcd4</t>
+  </si>
+  <si>
+    <t>0.69</t>
+  </si>
+  <si>
+    <t>000000000005</t>
+  </si>
+  <si>
+    <t>Jupi Yufi</t>
+  </si>
+  <si>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>000000000006</t>
+  </si>
+  <si>
+    <t>Zixe Gevu</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>000000000007</t>
+  </si>
+  <si>
+    <t>Cado Nopo</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
     <t>000000000008</t>
   </si>
   <si>
-    <t>abcd3</t>
-  </si>
-  <si>
-    <t>1500.0</t>
-  </si>
-  <si>
-    <t>2023-02-22</t>
-  </si>
-  <si>
-    <t>000000000009</t>
-  </si>
-  <si>
-    <t>abcd4</t>
-  </si>
-  <si>
-    <t>1200.0</t>
-  </si>
-  <si>
-    <t>000000000010</t>
-  </si>
-  <si>
-    <t>Pojo Hoqo</t>
-  </si>
-  <si>
-    <t>1910.0</t>
-  </si>
-  <si>
-    <t>000000000011</t>
-  </si>
-  <si>
-    <t>Teli Kezo</t>
-  </si>
-  <si>
-    <t>1150.0</t>
-  </si>
-  <si>
-    <t>000000000012</t>
-  </si>
-  <si>
-    <t>Husu Toqa</t>
-  </si>
-  <si>
-    <t>1040.0</t>
-  </si>
-  <si>
-    <t>000000000013</t>
-  </si>
-  <si>
-    <t>Sexo Nuyo</t>
-  </si>
-  <si>
-    <t>1170.0</t>
-  </si>
-  <si>
-    <t>000000000014</t>
-  </si>
-  <si>
-    <t>Dibo Xibu</t>
-  </si>
-  <si>
-    <t>1130.0</t>
-  </si>
-  <si>
-    <t>000000000015</t>
-  </si>
-  <si>
-    <t>Gepu Yigo</t>
-  </si>
-  <si>
-    <t>1320.0</t>
-  </si>
-  <si>
-    <t>000000000016</t>
-  </si>
-  <si>
-    <t>Vapu Jixa</t>
-  </si>
-  <si>
-    <t>1090.0</t>
-  </si>
-  <si>
-    <t>000000000017</t>
-  </si>
-  <si>
-    <t>Kanu Poza</t>
-  </si>
-  <si>
-    <t>1080.0</t>
-  </si>
-  <si>
-    <t>000000000000</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>1060.0</t>
-  </si>
-  <si>
-    <t>000000000018</t>
-  </si>
-  <si>
-    <t>Niki Cela</t>
-  </si>
-  <si>
-    <t>1690.0</t>
-  </si>
-  <si>
-    <t>000000000019</t>
-  </si>
-  <si>
-    <t>Lisi Kimi</t>
-  </si>
-  <si>
-    <t>1830.0</t>
-  </si>
-  <si>
-    <t>000000000001</t>
-  </si>
-  <si>
-    <t>abcd1</t>
-  </si>
-  <si>
-    <t>000000000002</t>
-  </si>
-  <si>
-    <t>abcd2</t>
-  </si>
-  <si>
-    <t>000000000003</t>
-  </si>
-  <si>
-    <t>000000000004</t>
-  </si>
-  <si>
-    <t>1850.0</t>
-  </si>
-  <si>
-    <t>000000000005</t>
-  </si>
-  <si>
-    <t>1230.0</t>
-  </si>
-  <si>
-    <t>000000000006</t>
-  </si>
-  <si>
-    <t>1070.0</t>
-  </si>
-  <si>
-    <t>000000000007</t>
-  </si>
-  <si>
-    <t>1250.0</t>
+    <t>Gasu Haro</t>
+  </si>
+  <si>
+    <t>0.11</t>
   </si>
 </sst>
 </file>
@@ -227,7 +242,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -437,7 +452,7 @@
         <v>45</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s" s="0">
         <v>7</v>
@@ -445,13 +460,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s" s="0">
         <v>7</v>
@@ -459,13 +474,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s" s="0">
         <v>7</v>
@@ -473,13 +488,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s" s="0">
         <v>7</v>
@@ -487,13 +502,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s" s="0">
         <v>7</v>
@@ -501,29 +516,15 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="D21" t="s" s="0">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
unused packeages removed and formatting resolved
</commit_message>
<xml_diff>
--- a/cusaccount.xlsx
+++ b/cusaccount.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Account Id</t>
   </si>
@@ -29,10 +29,10 @@
     <t>000000000009</t>
   </si>
   <si>
-    <t>Giza Venu</t>
-  </si>
-  <si>
-    <t>1080.0</t>
+    <t>Laba Bubi</t>
+  </si>
+  <si>
+    <t>1770.0</t>
   </si>
   <si>
     <t>2023-02-24</t>
@@ -41,127 +41,121 @@
     <t>000000000010</t>
   </si>
   <si>
-    <t>Rifa Kuca</t>
-  </si>
-  <si>
-    <t>1870.0</t>
+    <t>Tifu Fubu</t>
+  </si>
+  <si>
+    <t>1060.0</t>
   </si>
   <si>
     <t>000000000011</t>
   </si>
   <si>
-    <t>Hura Digi</t>
+    <t>Mive Miwu</t>
+  </si>
+  <si>
+    <t>1610.0</t>
+  </si>
+  <si>
+    <t>000000000012</t>
+  </si>
+  <si>
+    <t>Ceti Beqo</t>
+  </si>
+  <si>
+    <t>1130.0</t>
+  </si>
+  <si>
+    <t>000000000013</t>
+  </si>
+  <si>
+    <t>Dihi Lare</t>
+  </si>
+  <si>
+    <t>1290.0</t>
+  </si>
+  <si>
+    <t>000000000014</t>
+  </si>
+  <si>
+    <t>Tavi Mihi</t>
+  </si>
+  <si>
+    <t>1520.0</t>
+  </si>
+  <si>
+    <t>000000000015</t>
+  </si>
+  <si>
+    <t>Gone Kuca</t>
+  </si>
+  <si>
+    <t>1480.0</t>
+  </si>
+  <si>
+    <t>000000000016</t>
+  </si>
+  <si>
+    <t>Cevu Xuxi</t>
+  </si>
+  <si>
+    <t>1910.0</t>
+  </si>
+  <si>
+    <t>000000000017</t>
+  </si>
+  <si>
+    <t>Mupu Viba</t>
+  </si>
+  <si>
+    <t>1540.0</t>
+  </si>
+  <si>
+    <t>000000000018</t>
+  </si>
+  <si>
+    <t>Rufa Coqi</t>
+  </si>
+  <si>
+    <t>1330.0</t>
+  </si>
+  <si>
+    <t>000000000001</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>000000000019</t>
+  </si>
+  <si>
+    <t>Neka Jopo</t>
+  </si>
+  <si>
+    <t>000000000002</t>
+  </si>
+  <si>
+    <t>abcd1</t>
+  </si>
+  <si>
+    <t>1890.0</t>
+  </si>
+  <si>
+    <t>000000000003</t>
+  </si>
+  <si>
+    <t>abcd2</t>
   </si>
   <si>
     <t>1550.0</t>
   </si>
   <si>
-    <t>000000000012</t>
-  </si>
-  <si>
-    <t>Vile Qoxu</t>
-  </si>
-  <si>
-    <t>1130.0</t>
-  </si>
-  <si>
-    <t>000000000013</t>
-  </si>
-  <si>
-    <t>Wadu Raro</t>
-  </si>
-  <si>
-    <t>1760.0</t>
-  </si>
-  <si>
-    <t>000000000014</t>
-  </si>
-  <si>
-    <t>Sopu Dugi</t>
-  </si>
-  <si>
-    <t>1420.0</t>
-  </si>
-  <si>
-    <t>000000000015</t>
-  </si>
-  <si>
-    <t>Vuze Piwi</t>
-  </si>
-  <si>
-    <t>1490.0</t>
-  </si>
-  <si>
-    <t>000000000016</t>
-  </si>
-  <si>
-    <t>Cebu Napo</t>
-  </si>
-  <si>
-    <t>1020.0</t>
-  </si>
-  <si>
-    <t>000000000017</t>
-  </si>
-  <si>
-    <t>Wonu Bejo</t>
-  </si>
-  <si>
-    <t>1220.0</t>
-  </si>
-  <si>
-    <t>000000000018</t>
-  </si>
-  <si>
-    <t>Yiqo Puyi</t>
-  </si>
-  <si>
-    <t>1770.0</t>
-  </si>
-  <si>
-    <t>000000000001</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>1190.0</t>
-  </si>
-  <si>
-    <t>000000000019</t>
-  </si>
-  <si>
-    <t>Piyo Noju</t>
-  </si>
-  <si>
-    <t>1590.0</t>
-  </si>
-  <si>
-    <t>000000000002</t>
-  </si>
-  <si>
-    <t>abcd1</t>
-  </si>
-  <si>
-    <t>1540.0</t>
-  </si>
-  <si>
-    <t>000000000003</t>
-  </si>
-  <si>
-    <t>abcd2</t>
-  </si>
-  <si>
-    <t>1630.0</t>
-  </si>
-  <si>
     <t>000000000004</t>
   </si>
   <si>
     <t>abcd3</t>
   </si>
   <si>
-    <t>1210.0</t>
+    <t>1900.0</t>
   </si>
   <si>
     <t>000000000005</t>
@@ -170,34 +164,34 @@
     <t>abcd4</t>
   </si>
   <si>
-    <t>1680.0</t>
+    <t>1370.0</t>
   </si>
   <si>
     <t>000000000006</t>
   </si>
   <si>
-    <t>Qohu Vusa</t>
-  </si>
-  <si>
-    <t>1500.0</t>
+    <t>Dire Wati</t>
+  </si>
+  <si>
+    <t>1140.0</t>
   </si>
   <si>
     <t>000000000007</t>
   </si>
   <si>
-    <t>Raqa Baki</t>
-  </si>
-  <si>
-    <t>1620.0</t>
+    <t>Xehi Vuhi</t>
+  </si>
+  <si>
+    <t>1180.0</t>
   </si>
   <si>
     <t>000000000008</t>
   </si>
   <si>
-    <t>Jiwo Wapo</t>
-  </si>
-  <si>
-    <t>2000.0</t>
+    <t>Bica Lije</t>
+  </si>
+  <si>
+    <t>1390.0</t>
   </si>
 </sst>
 </file>
@@ -410,7 +404,7 @@
         <v>36</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s" s="0">
         <v>7</v>
@@ -418,13 +412,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B13" t="s" s="0">
-        <v>39</v>
-      </c>
       <c r="C13" t="s" s="0">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s" s="0">
         <v>7</v>
@@ -432,13 +426,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s" s="0">
         <v>41</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>43</v>
       </c>
       <c r="D14" t="s" s="0">
         <v>7</v>
@@ -446,13 +440,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s" s="0">
         <v>44</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>46</v>
       </c>
       <c r="D15" t="s" s="0">
         <v>7</v>
@@ -460,13 +454,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s" s="0">
         <v>47</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>49</v>
       </c>
       <c r="D16" t="s" s="0">
         <v>7</v>
@@ -474,13 +468,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s" s="0">
         <v>50</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="C17" t="s" s="0">
-        <v>52</v>
       </c>
       <c r="D17" t="s" s="0">
         <v>7</v>
@@ -488,13 +482,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s" s="0">
         <v>53</v>
-      </c>
-      <c r="B18" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>55</v>
       </c>
       <c r="D18" t="s" s="0">
         <v>7</v>
@@ -502,13 +496,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s" s="0">
         <v>56</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="C19" t="s" s="0">
-        <v>58</v>
       </c>
       <c r="D19" t="s" s="0">
         <v>7</v>
@@ -516,13 +510,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s" s="0">
         <v>59</v>
-      </c>
-      <c r="B20" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="C20" t="s" s="0">
-        <v>61</v>
       </c>
       <c r="D20" t="s" s="0">
         <v>7</v>

</xml_diff>